<commit_message>
Add database integration and path normalization
- Add db_export module for saving valuations to SQLite database
- Integrate DB save into CLI (main.py) and web app (web_app.py)
- Add adjusted_price_reporting (reverse forex) to gap analysis
- Normalize output directory path: Stock_valuation → stock_valuation
- Update gap analysis display to show reporting currency values

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/modeling/DCF valuation template.xlsx
+++ b/modeling/DCF valuation template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alan/modeling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alan/ValuX/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E888562B-63EE-8848-AA59-CDBF0BC4006C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1B0DB3-1DBC-C045-9BE2-2A5D6765578C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="16140" xr2:uid="{CEA4A7B3-03C5-AA4D-8210-EE5C56A7CF9B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Year</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -55,10 +55,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>EBIT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>EBIT(1-t)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -249,6 +245,14 @@
   </si>
   <si>
     <t>WACC for forecast year 1-5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Operating Profit (EBIT)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Operating Profit (EBIT) margin</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -873,14 +877,14 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E1" s="21"/>
       <c r="F1" s="39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G1" s="39"/>
       <c r="H1" s="39"/>
@@ -895,7 +899,7 @@
     </row>
     <row r="2" spans="1:18" ht="19">
       <c r="A2" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>2024</v>
@@ -952,11 +956,11 @@
     </row>
     <row r="3" spans="1:18" ht="16" customHeight="1">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="24"/>
       <c r="D3" s="37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="26">
         <f>E4-1%</f>
@@ -1001,7 +1005,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="36"/>
       <c r="D4" s="37"/>
@@ -1047,7 +1051,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="36"/>
       <c r="D5" s="37"/>
@@ -1093,7 +1097,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="36"/>
       <c r="D6" s="37"/>
@@ -1139,7 +1143,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="26">
@@ -1184,7 +1188,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="26">
@@ -1228,7 +1232,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="26">
@@ -1273,7 +1277,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="26">
@@ -1318,7 +1322,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="24"/>
       <c r="D11" s="37"/>
@@ -1364,7 +1368,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="24"/>
       <c r="D12" s="37"/>
@@ -1410,7 +1414,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="23"/>
       <c r="D13" s="38"/>
@@ -1456,7 +1460,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="24"/>
       <c r="D14" s="29"/>
@@ -1494,34 +1498,34 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="24"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1"/>
       <c r="E17" s="24"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1"/>
       <c r="E18" s="24"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="1"/>
       <c r="E19" s="24"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="24"/>
     </row>
@@ -1546,7 +1550,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1561,7 +1565,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="15">
         <v>1</v>
@@ -1594,7 +1598,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="8" customFormat="1">
@@ -1749,7 +1753,7 @@
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1">
       <c r="A5" s="4" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="B5" s="10" t="e">
         <f>B6/B4</f>
@@ -1802,7 +1806,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="4" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11">
@@ -1852,7 +1856,7 @@
     </row>
     <row r="7" spans="1:13" s="1" customFormat="1">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="12">
         <f>'Input and sensitivity'!B14</f>
@@ -1905,7 +1909,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="11">
         <f>B6*(1-B7)</f>
@@ -1958,7 +1962,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="4">
         <f>IF(C32=0,0,IF(C4&gt;B4,(C4-B4)/C32,0))</f>
@@ -2007,7 +2011,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="6">
         <f>B8-B9</f>
@@ -2060,7 +2064,7 @@
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1">
       <c r="A12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="13">
         <f>'Input and sensitivity'!B11</f>
@@ -2113,7 +2117,7 @@
     </row>
     <row r="13" spans="1:13" s="2" customFormat="1">
       <c r="A13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="2">
         <f>1/(1+C12)^1</f>
@@ -2158,7 +2162,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6">
@@ -2208,7 +2212,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="4">
         <f>M10</f>
@@ -2217,7 +2221,7 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="3">
         <f>M12</f>
@@ -2226,7 +2230,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="4" t="e">
         <f>B16/(B17-M3)</f>
@@ -2235,7 +2239,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="4" t="e">
         <f>B18*L13</f>
@@ -2248,7 +2252,7 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="4">
         <f>SUM(C14:L14)</f>
@@ -2261,7 +2265,7 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4" t="e">
         <f>B20+B19</f>
@@ -2270,19 +2274,19 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="11"/>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="11"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="11" t="e">
         <f>B21+B22+B23</f>
@@ -2291,19 +2295,19 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="11"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="11"/>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" s="11" t="e">
         <f>B24-B25-B26</f>
@@ -2312,13 +2316,13 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="11"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B29" s="9" t="e">
         <f>B27/B28*1000000</f>
@@ -2327,7 +2331,7 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -2344,7 +2348,7 @@
     </row>
     <row r="32" spans="1:13" s="11" customFormat="1">
       <c r="A32" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="16" t="e">
         <f>B4/B33</f>
@@ -2394,7 +2398,7 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="4">
@@ -2440,7 +2444,7 @@
     </row>
     <row r="34" spans="1:13" s="3" customFormat="1">
       <c r="A34" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="3" t="e">
         <f t="shared" ref="B34:L34" si="15">B8/B33</f>
@@ -2493,7 +2497,7 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="4">
         <f>'Input and sensitivity'!B7</f>

</xml_diff>